<commit_message>
Rename mmm -> tiled_mmm
</commit_message>
<xml_diff>
--- a/results/timing.xlsx
+++ b/results/timing.xlsx
@@ -825,13 +825,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -865,13 +868,13 @@
         <v>326</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C14" si="0">B3/A3</f>
+        <f t="shared" ref="C3:C18" si="0">B3/A3</f>
         <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <f t="shared" ref="A4:A15" si="1">A3*2</f>
+        <f t="shared" ref="A4:A18" si="1">A3*2</f>
         <v>4</v>
       </c>
       <c r="B4">
@@ -940,11 +943,11 @@
         <v>128</v>
       </c>
       <c r="B9">
-        <v>18857</v>
+        <v>18852</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>147.3203125</v>
+        <v>147.28125</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -953,11 +956,11 @@
         <v>256</v>
       </c>
       <c r="B10">
-        <v>38521</v>
+        <v>38506</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>150.47265625</v>
+        <v>150.4140625</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -966,11 +969,11 @@
         <v>512</v>
       </c>
       <c r="B11">
-        <v>78311</v>
+        <v>78276</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>152.951171875</v>
+        <v>152.8828125</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -979,11 +982,11 @@
         <v>1024</v>
       </c>
       <c r="B12">
-        <v>158584</v>
+        <v>158509</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>154.8671875</v>
+        <v>154.7939453125</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -992,23 +995,76 @@
         <v>2048</v>
       </c>
       <c r="B13">
-        <v>320558</v>
+        <v>320403</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>156.5224609375</v>
+        <v>156.44677734375</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
+        <f t="shared" si="1"/>
         <v>4096</v>
       </c>
       <c r="B14">
-        <v>647026</v>
+        <v>646711</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>157.96533203125</v>
+        <v>157.888427734375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>1304115</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>159.1937255859375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="B16">
+        <v>2629255</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>160.47698974609375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>32768</v>
+      </c>
+      <c r="B17">
+        <v>5132855</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>156.64230346679687</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="B18">
+        <v>10331339</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>157.64372253417969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>